<commit_message>
Adding vehicle scenarios part 1
</commit_message>
<xml_diff>
--- a/src/test/resources/credentials.xlsx
+++ b/src/test/resources/credentials.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="192" yWindow="48" windowWidth="28356" windowHeight="12192" activeTab="1"/>
+    <workbookView xWindow="192" yWindow="48" windowWidth="23256" windowHeight="12192" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CREDENTIALS" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>url.driver.qa</t>
   </si>
@@ -44,13 +44,25 @@
     <t>CXD7G2Ke5U!FHanVCzS</t>
   </si>
   <si>
-    <t>https://driver.qa1.mobile22.com</t>
-  </si>
-  <si>
-    <t>https://vehicle.qa1.mobile22.com</t>
-  </si>
-  <si>
-    <t>https://callcenter.qa1.mobile22.com</t>
+    <t>https://vehicle.dev.mobile22.com</t>
+  </si>
+  <si>
+    <t>username.2</t>
+  </si>
+  <si>
+    <t>password.2</t>
+  </si>
+  <si>
+    <t>sukanabec@mailinator.com</t>
+  </si>
+  <si>
+    <t>changeMe22@</t>
+  </si>
+  <si>
+    <t>https://driver.dev.mobile22.com</t>
+  </si>
+  <si>
+    <t>https://callcenter.dev.mobile22.com</t>
   </si>
 </sst>
 </file>
@@ -434,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -450,7 +462,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1"/>
     </row>
@@ -458,8 +470,8 @@
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
+      <c r="B2" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="C2" s="1"/>
     </row>
@@ -473,9 +485,27 @@
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId1"/>
+    <hyperlink ref="B1" r:id="rId2"/>
+    <hyperlink ref="B2" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -486,7 +516,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -508,7 +538,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -516,7 +546,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -524,7 +554,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding Sign up scenario in driver app
</commit_message>
<xml_diff>
--- a/src/test/resources/credentials.xlsx
+++ b/src/test/resources/credentials.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>url.driver.qa</t>
   </si>
@@ -63,6 +63,12 @@
   </si>
   <si>
     <t>https://callcenter.dev.mobile22.com</t>
+  </si>
+  <si>
+    <t>url.driverapp.qa</t>
+  </si>
+  <si>
+    <t>https://driverapp.dev.mobile22.com</t>
   </si>
 </sst>
 </file>
@@ -513,10 +519,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -525,7 +531,7 @@
     <col min="2" max="2" width="31.44140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -533,7 +539,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -541,29 +547,44 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C6" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="B3" r:id="rId2"/>
     <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId4"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding new fare test - part 1
</commit_message>
<xml_diff>
--- a/src/test/resources/credentials.xlsx
+++ b/src/test/resources/credentials.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RamonPC\Desktop\Ramon\Workspace_mobile22\QAWebAutomation\src\test\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D042818-BF3B-456E-9F6E-194EB38FE66D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="192" yWindow="48" windowWidth="23256" windowHeight="12192" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CREDENTIALS" sheetId="2" r:id="rId1"/>
@@ -15,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>url.driver.qa</t>
   </si>
@@ -69,13 +75,28 @@
   </si>
   <si>
     <t>https://driverapp.dev.mobile22.com</t>
+  </si>
+  <si>
+    <t>url.uat.rides</t>
+  </si>
+  <si>
+    <t>https://rides.uat.mobile22.com/</t>
+  </si>
+  <si>
+    <t>username.3</t>
+  </si>
+  <si>
+    <t>vango@mailinator.com</t>
+  </si>
+  <si>
+    <t>password.3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,6 +116,27 @@
     <font>
       <u/>
       <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -139,21 +181,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+  <cellStyles count="4">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink 2" xfId="3" xr:uid="{6E0B4DDD-A72B-47CF-A641-DDB4942E3481}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{B22E5C25-6876-42A8-AFDA-9B3BFF275AE6}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -161,12 +209,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -208,7 +259,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -241,9 +292,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -276,6 +344,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -451,14 +536,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="26.5546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -507,25 +592,44 @@
         <v>8</v>
       </c>
     </row>
+    <row r="11" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
-    <hyperlink ref="B1" r:id="rId2"/>
-    <hyperlink ref="B2" r:id="rId3"/>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B1" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B11" r:id="rId4" xr:uid="{A692F2D8-E3BE-274E-8F53-5EF5E97F26A1}"/>
+    <hyperlink ref="B12" r:id="rId5" xr:uid="{422E7BF5-BF47-7E41-B4D0-3BDB8600A22E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.44140625" style="1" bestFit="1" customWidth="1"/>
@@ -575,14 +679,20 @@
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="C6" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId5"/>

</xml_diff>